<commit_message>
updated derived files and Rmd file
</commit_message>
<xml_diff>
--- a/data/derived/2020-04-21_air-dry-2019-whc/air-dry-2019-whc_2020-04-21.xlsx
+++ b/data/derived/2020-04-21_air-dry-2019-whc/air-dry-2019-whc_2020-04-21.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="24880" windowHeight="16740" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="24880" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -701,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1880,7 +1880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>